<commit_message>
Schedule changes, local info
</commit_message>
<xml_diff>
--- a/ANITA 2022 school and workshop registration (Responses).xlsx
+++ b/ANITA 2022 school and workshop registration (Responses).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyam/Work/ASA/ANITA/workshop2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C476342-DA90-D94A-A80E-9361EA91F535}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DA7C82-6BB4-154B-81E6-D9ECA05FB254}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2180" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -37,7 +37,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="K32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="I45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="J45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="H52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="I52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -133,13 +133,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="K52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -689,12 +690,6 @@
     <t>Cinquegrana</t>
   </si>
   <si>
-    <t>The initial mass for CC SNe in the most metal-rich regions of the universe</t>
-  </si>
-  <si>
-    <t>coeliac</t>
-  </si>
-  <si>
     <t>amit.seta@anu.edu.au</t>
   </si>
   <si>
@@ -978,6 +973,12 @@
   </si>
   <si>
     <t>National Research Council of Canada</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>coeliac -&gt; switched to remote</t>
   </si>
 </sst>
 </file>
@@ -987,7 +988,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -997,6 +998,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1019,11 +1032,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1245,8 +1260,8 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1378,182 +1393,161 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>44515.868023379633</v>
+        <v>44565.455088773146</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>44567.593295590283</v>
+        <v>44516.461602523152</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>137</v>
+        <v>17</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>44517.943335150463</v>
+        <v>44517.437605879633</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>143</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>44518.674947118052</v>
+        <v>44518.522700555557</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>44538.65844013889</v>
+        <v>44538.734623819444</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>182</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <v>44538.658461423613</v>
+        <v>44538.749987280091</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>185</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>187</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>64</v>
@@ -1565,30 +1559,27 @@
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>44538.664243425927</v>
+        <v>44546.425724270834</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>190</v>
+        <v>85</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>15</v>
@@ -1597,33 +1588,30 @@
         <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>193</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>44539.359042777782</v>
+        <v>44547.518509270834</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>210</v>
+        <v>87</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>211</v>
+        <v>88</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>212</v>
+        <v>89</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>213</v>
+        <v>42</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
@@ -1632,234 +1620,207 @@
         <v>16</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>214</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>44577.536283645837</v>
+        <v>44553.359632361113</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>266</v>
+        <v>94</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>267</v>
+        <v>95</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>268</v>
+        <v>96</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>269</v>
+        <v>97</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>270</v>
+        <v>17</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>271</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>44523.144790243052</v>
+        <v>44554.049739050926</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>44524.591511828708</v>
+        <v>44542.011398217597</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>44538.714371377311</v>
+        <v>44516.697951863425</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>205</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>206</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>207</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>208</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>44539.464385092593</v>
+        <v>44516.698097974542</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>220</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>222</v>
+        <v>33</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>223</v>
+        <v>34</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>224</v>
+        <v>17</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>44565.982171990741</v>
+        <v>44516.818202523151</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>246</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>247</v>
+        <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>248</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>249</v>
+        <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>44575.71996800926</v>
+        <v>44538.663162314813</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>256</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>257</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>258</v>
+        <v>52</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>15</v>
@@ -1868,419 +1829,416 @@
         <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>259</v>
+        <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
-        <v>44567.593282523143</v>
+        <v>44538.710119918978</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>260</v>
+        <v>53</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>262</v>
+        <v>55</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>263</v>
+        <v>56</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>264</v>
+        <v>17</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>265</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
-        <v>44565.663936550925</v>
+        <v>44539.574667499997</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>272</v>
+        <v>65</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>273</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>274</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>275</v>
+        <v>60</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="H21" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="J21" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
-        <v>44565.455088773146</v>
+        <v>44540.64818452546</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
-        <v>44516.461602523152</v>
+        <v>44543.919701145831</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
-        <v>44517.437605879633</v>
+        <v>44545.69106542824</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
-        <v>44518.522700555557</v>
+        <v>44548.898509432867</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
-        <v>44538.734623819444</v>
+        <v>44565.649739212968</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
-        <v>44538.749987280091</v>
+        <v>44566.573276030089</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
-        <v>44546.425724270834</v>
+        <v>44566.670522870365</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
-        <v>44547.518509270834</v>
+        <v>44572.566709872684</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
-        <v>44553.359632361113</v>
+        <v>44574.658028379628</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <v>44554.049739050926</v>
+        <v>44515.868023379633</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
-        <v>44542.011398217597</v>
+      <c r="A32" s="4">
+        <v>44567.593295590283</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2">
-        <v>44516.620116099541</v>
+      <c r="A33" s="4">
+        <v>44517.943335150463</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>17</v>
@@ -2292,30 +2250,33 @@
         <v>15</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2">
-        <v>44546.509251076393</v>
+      <c r="A34" s="4">
+        <v>44518.674947118052</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>16</v>
@@ -2324,27 +2285,27 @@
         <v>15</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2">
-        <v>44523.476997465274</v>
+      <c r="A35" s="4">
+        <v>44538.65844013889</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>17</v>
@@ -2356,27 +2317,27 @@
         <v>15</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2">
-        <v>44526.44112260417</v>
+      <c r="A36" s="4">
+        <v>44538.658461423613</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>15</v>
@@ -2388,24 +2349,24 @@
         <v>15</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2">
-        <v>44538.394358391204</v>
+      <c r="A37" s="4">
+        <v>44538.664243425927</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>116</v>
@@ -2420,30 +2381,33 @@
         <v>15</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
-        <v>44547.511355300929</v>
+        <v>44539.359042777782</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>16</v>
@@ -2452,30 +2416,30 @@
         <v>15</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
-        <v>44540.515796087959</v>
+        <v>44577.536283645837</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>42</v>
+        <v>267</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
@@ -2487,564 +2451,624 @@
         <v>15</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
-        <v>44544.587308518516</v>
+        <v>44523.144790243052</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>239</v>
+        <v>152</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
-        <v>44547.600391053245</v>
+        <v>44524.591511828708</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>242</v>
+        <v>162</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>243</v>
+        <v>163</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>244</v>
+        <v>164</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>245</v>
+        <v>166</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
-        <v>44516.697951863425</v>
+        <v>44538.714371377311</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>28</v>
+        <v>204</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
-        <v>44516.698097974542</v>
+        <v>44539.464385092593</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>31</v>
+        <v>218</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>32</v>
+        <v>219</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>34</v>
+        <v>221</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
-        <v>44516.818202523151</v>
+        <v>44565.982171990741</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>35</v>
+        <v>244</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>36</v>
+        <v>245</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>37</v>
+        <v>246</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
-        <v>44538.663162314813</v>
+        <v>44575.71996800926</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>51</v>
+        <v>255</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>52</v>
+        <v>256</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="4">
+        <v>44567.593282523143</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="4">
+        <v>44516.620116099541</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="4">
+        <v>44546.509251076393</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2">
-        <v>44538.710119918978</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2">
-        <v>44539.574667499997</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="F48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="4">
+        <v>44523.476997465274</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A50" s="4">
+        <v>44526.44112260417</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2">
-        <v>44540.64818452546</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2">
-        <v>44543.919701145831</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="2">
-        <v>44545.69106542824</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="F50" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="2">
-        <v>44548.898509432867</v>
+      <c r="A51" s="4">
+        <v>44538.394358391204</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>90</v>
+        <v>172</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="2">
-        <v>44565.649739212968</v>
+      <c r="A52" s="4">
+        <v>44547.511355300929</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="E52" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="4">
+        <v>44540.515796087959</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="4">
+        <v>44544.587308518516</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="2">
-        <v>44566.573276030089</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="2">
-        <v>44566.670522870365</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="F54" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="2">
-        <v>44572.566709872684</v>
+      <c r="A55" s="4">
+        <v>44547.600391053245</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>118</v>
+        <v>241</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>119</v>
+        <v>242</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="2">
-        <v>44574.658028379628</v>
+      <c r="A56" s="4">
+        <v>44540.545156284723</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>121</v>
+        <v>232</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>122</v>
+        <v>233</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="K56" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="2">
-        <v>44540.545156284723</v>
+      <c r="A57" s="4">
+        <v>44538.688029490746</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>22</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="2">
-        <v>44538.688029490746</v>
+      <c r="A58" s="4">
+        <v>44538.707016875</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>15</v>
@@ -3056,30 +3080,27 @@
         <v>15</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K58" s="3" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="59" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="2">
-        <v>44538.707016875</v>
+      <c r="A59" s="4">
+        <v>44539.395467361115</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>15</v>
@@ -3091,27 +3112,30 @@
         <v>15</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
-        <v>44539.395467361115</v>
+        <v>44539.514666736111</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>15</v>
@@ -3123,30 +3147,30 @@
         <v>15</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>22</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
-        <v>44539.514666736111</v>
+        <v>44566.507624618054</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>15</v>
@@ -3158,27 +3182,24 @@
         <v>15</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
-        <v>44566.507624618054</v>
+        <v>44567.098108668986</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>136</v>
@@ -3193,52 +3214,47 @@
         <v>15</v>
       </c>
       <c r="I62" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
-        <v>44567.098108668986</v>
+        <v>44565.663936550925</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>136</v>
+        <v>273</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="J63" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>255</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:K63">
-    <sortCondition ref="J2:J63"/>
+    <sortCondition ref="H2:H63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>